<commit_message>
version as of Jan 16
</commit_message>
<xml_diff>
--- a/2023 Report/margin_per_game.xlsx
+++ b/2023 Report/margin_per_game.xlsx
@@ -1,15 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27510"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Brenton/Documents/Fantasy-Football/2023 Report/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="19260" windowHeight="14300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -166,8 +179,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,6 +243,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -276,12 +294,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -308,14 +326,15 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -342,6 +361,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -517,14 +537,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K281"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A189" workbookViewId="0">
+      <selection activeCell="H231" sqref="H231"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -556,7 +578,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -582,7 +604,7 @@
         <v>178.8</v>
       </c>
       <c r="I2">
-        <v>0.0400000000000063</v>
+        <v>4.0000000000006301E-2</v>
       </c>
       <c r="J2" t="s">
         <v>33</v>
@@ -591,7 +613,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -626,7 +648,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -661,7 +683,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -696,7 +718,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -722,7 +744,7 @@
         <v>189.38</v>
       </c>
       <c r="I6">
-        <v>0.420000000000002</v>
+        <v>0.42000000000000198</v>
       </c>
       <c r="J6" t="s">
         <v>36</v>
@@ -731,7 +753,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -757,7 +779,7 @@
         <v>232.64</v>
       </c>
       <c r="I7">
-        <v>0.480000000000004</v>
+        <v>0.48000000000000398</v>
       </c>
       <c r="J7" t="s">
         <v>37</v>
@@ -766,7 +788,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -792,7 +814,7 @@
         <v>248.66</v>
       </c>
       <c r="I8">
-        <v>0.700000000000003</v>
+        <v>0.70000000000000295</v>
       </c>
       <c r="J8" t="s">
         <v>38</v>
@@ -801,7 +823,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -827,7 +849,7 @@
         <v>243.76</v>
       </c>
       <c r="I9">
-        <v>0.719999999999999</v>
+        <v>0.71999999999999897</v>
       </c>
       <c r="J9" t="s">
         <v>39</v>
@@ -836,7 +858,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -871,7 +893,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -906,7 +928,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -941,7 +963,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -976,7 +998,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1011,7 +1033,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1046,7 +1068,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1081,7 +1103,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1116,7 +1138,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1151,7 +1173,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1186,7 +1208,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1212,7 +1234,7 @@
         <v>221.08</v>
       </c>
       <c r="I20">
-        <v>2.44000000000001</v>
+        <v>2.4400000000000102</v>
       </c>
       <c r="J20" t="s">
         <v>36</v>
@@ -1221,7 +1243,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1247,7 +1269,7 @@
         <v>229.46</v>
       </c>
       <c r="I21">
-        <v>2.54000000000001</v>
+        <v>2.5400000000000098</v>
       </c>
       <c r="J21" t="s">
         <v>39</v>
@@ -1256,7 +1278,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1291,7 +1313,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1326,7 +1348,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1361,7 +1383,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1396,7 +1418,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1431,7 +1453,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1466,7 +1488,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1489,10 +1511,10 @@
         <v>142.46</v>
       </c>
       <c r="H28">
-        <v>287.96</v>
+        <v>287.95999999999998</v>
       </c>
       <c r="I28">
-        <v>3.03999999999999</v>
+        <v>3.0399999999999898</v>
       </c>
       <c r="J28" t="s">
         <v>45</v>
@@ -1501,7 +1523,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1536,7 +1558,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1571,7 +1593,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1606,7 +1628,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1641,7 +1663,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1667,7 +1689,7 @@
         <v>232.9</v>
       </c>
       <c r="I33">
-        <v>3.53999999999999</v>
+        <v>3.5399999999999898</v>
       </c>
       <c r="J33" t="s">
         <v>47</v>
@@ -1676,7 +1698,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1711,7 +1733,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1737,7 +1759,7 @@
         <v>196.68</v>
       </c>
       <c r="I35">
-        <v>3.59999999999999</v>
+        <v>3.5999999999999899</v>
       </c>
       <c r="J35" t="s">
         <v>45</v>
@@ -1746,7 +1768,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1781,7 +1803,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1798,16 +1820,16 @@
         <v>17</v>
       </c>
       <c r="F37">
-        <v>146.48</v>
+        <v>146.47999999999999</v>
       </c>
       <c r="G37">
         <v>142.56</v>
       </c>
       <c r="H37">
-        <v>289.04</v>
+        <v>289.04000000000002</v>
       </c>
       <c r="I37">
-        <v>3.91999999999999</v>
+        <v>3.9199999999999902</v>
       </c>
       <c r="J37" t="s">
         <v>36</v>
@@ -1816,7 +1838,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1851,7 +1873,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1877,7 +1899,7 @@
         <v>237.36</v>
       </c>
       <c r="I39">
-        <v>4.32000000000001</v>
+        <v>4.3200000000000101</v>
       </c>
       <c r="J39" t="s">
         <v>34</v>
@@ -1886,7 +1908,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1906,13 +1928,13 @@
         <v>137.22</v>
       </c>
       <c r="G40">
-        <v>132.86</v>
+        <v>132.86000000000001</v>
       </c>
       <c r="H40">
         <v>270.08</v>
       </c>
       <c r="I40">
-        <v>4.35999999999999</v>
+        <v>4.3599999999999897</v>
       </c>
       <c r="J40" t="s">
         <v>34</v>
@@ -1921,7 +1943,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1956,7 +1978,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1982,7 +2004,7 @@
         <v>171.06</v>
       </c>
       <c r="I42">
-        <v>4.69999999999999</v>
+        <v>4.6999999999999904</v>
       </c>
       <c r="J42" t="s">
         <v>38</v>
@@ -1991,7 +2013,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -2026,7 +2048,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -2052,7 +2074,7 @@
         <v>204.92</v>
       </c>
       <c r="I44">
-        <v>4.95999999999999</v>
+        <v>4.9599999999999902</v>
       </c>
       <c r="J44" t="s">
         <v>36</v>
@@ -2061,7 +2083,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -2087,7 +2109,7 @@
         <v>182.66</v>
       </c>
       <c r="I45">
-        <v>5.46000000000001</v>
+        <v>5.4600000000000097</v>
       </c>
       <c r="J45" t="s">
         <v>42</v>
@@ -2096,7 +2118,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -2122,7 +2144,7 @@
         <v>186.08</v>
       </c>
       <c r="I46">
-        <v>5.60000000000001</v>
+        <v>5.6000000000000103</v>
       </c>
       <c r="J46" t="s">
         <v>38</v>
@@ -2131,7 +2153,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -2157,7 +2179,7 @@
         <v>258.3</v>
       </c>
       <c r="I47">
-        <v>5.82000000000001</v>
+        <v>5.8200000000000101</v>
       </c>
       <c r="J47" t="s">
         <v>42</v>
@@ -2166,7 +2188,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -2201,7 +2223,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -2227,7 +2249,7 @@
         <v>228.2</v>
       </c>
       <c r="I49">
-        <v>5.95999999999999</v>
+        <v>5.9599999999999902</v>
       </c>
       <c r="J49" t="s">
         <v>40</v>
@@ -2236,7 +2258,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:11">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -2262,7 +2284,7 @@
         <v>186.14</v>
       </c>
       <c r="I50">
-        <v>6.45999999999999</v>
+        <v>6.4599999999999902</v>
       </c>
       <c r="J50" t="s">
         <v>33</v>
@@ -2271,7 +2293,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -2297,7 +2319,7 @@
         <v>170.54</v>
       </c>
       <c r="I51">
-        <v>6.54000000000001</v>
+        <v>6.5400000000000098</v>
       </c>
       <c r="J51" t="s">
         <v>41</v>
@@ -2306,7 +2328,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -2329,10 +2351,10 @@
         <v>134.18</v>
       </c>
       <c r="H52">
-        <v>275.22</v>
+        <v>275.22000000000003</v>
       </c>
       <c r="I52">
-        <v>6.85999999999999</v>
+        <v>6.8599999999999897</v>
       </c>
       <c r="J52" t="s">
         <v>45</v>
@@ -2341,7 +2363,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -2376,7 +2398,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="54" spans="1:11">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -2402,7 +2424,7 @@
         <v>258.8</v>
       </c>
       <c r="I54">
-        <v>7.39999999999999</v>
+        <v>7.3999999999999897</v>
       </c>
       <c r="J54" t="s">
         <v>39</v>
@@ -2411,7 +2433,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="55" spans="1:11">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -2431,7 +2453,7 @@
         <v>83.84</v>
       </c>
       <c r="G55">
-        <v>76.4</v>
+        <v>76.400000000000006</v>
       </c>
       <c r="H55">
         <v>160.24</v>
@@ -2446,7 +2468,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="56" spans="1:11">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -2472,7 +2494,7 @@
         <v>210.04</v>
       </c>
       <c r="I56">
-        <v>7.67999999999999</v>
+        <v>7.6799999999999899</v>
       </c>
       <c r="J56" t="s">
         <v>40</v>
@@ -2481,7 +2503,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="57" spans="1:11">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -2507,7 +2529,7 @@
         <v>220.04</v>
       </c>
       <c r="I57">
-        <v>7.76000000000001</v>
+        <v>7.7600000000000096</v>
       </c>
       <c r="J57" t="s">
         <v>39</v>
@@ -2516,7 +2538,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="1:11">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -2533,7 +2555,7 @@
         <v>10</v>
       </c>
       <c r="F58">
-        <v>81.54</v>
+        <v>81.540000000000006</v>
       </c>
       <c r="G58">
         <v>73.5</v>
@@ -2542,7 +2564,7 @@
         <v>155.04</v>
       </c>
       <c r="I58">
-        <v>8.04000000000001</v>
+        <v>8.0400000000000098</v>
       </c>
       <c r="J58" t="s">
         <v>41</v>
@@ -2551,7 +2573,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="59" spans="1:11">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -2577,7 +2599,7 @@
         <v>219.88</v>
       </c>
       <c r="I59">
-        <v>8.2</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="J59" t="s">
         <v>47</v>
@@ -2586,7 +2608,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="60" spans="1:11">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -2612,7 +2634,7 @@
         <v>221.62</v>
       </c>
       <c r="I60">
-        <v>8.25999999999999</v>
+        <v>8.2599999999999891</v>
       </c>
       <c r="J60" t="s">
         <v>38</v>
@@ -2621,7 +2643,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="61" spans="1:11">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -2647,7 +2669,7 @@
         <v>239.58</v>
       </c>
       <c r="I61">
-        <v>8.66000000000001</v>
+        <v>8.6600000000000108</v>
       </c>
       <c r="J61" t="s">
         <v>35</v>
@@ -2656,7 +2678,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="62" spans="1:11">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -2682,7 +2704,7 @@
         <v>170.72</v>
       </c>
       <c r="I62">
-        <v>8.72</v>
+        <v>8.7200000000000006</v>
       </c>
       <c r="J62" t="s">
         <v>39</v>
@@ -2691,7 +2713,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="63" spans="1:11">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -2717,7 +2739,7 @@
         <v>213.08</v>
       </c>
       <c r="I63">
-        <v>8.8</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="J63" t="s">
         <v>40</v>
@@ -2726,7 +2748,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="64" spans="1:11">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -2743,7 +2765,7 @@
         <v>13</v>
       </c>
       <c r="F64">
-        <v>148.36</v>
+        <v>148.36000000000001</v>
       </c>
       <c r="G64">
         <v>139.5</v>
@@ -2752,7 +2774,7 @@
         <v>287.86</v>
       </c>
       <c r="I64">
-        <v>8.86000000000001</v>
+        <v>8.8600000000000101</v>
       </c>
       <c r="J64" t="s">
         <v>39</v>
@@ -2761,7 +2783,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="65" spans="1:11">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -2787,7 +2809,7 @@
         <v>207.48</v>
       </c>
       <c r="I65">
-        <v>8.95999999999999</v>
+        <v>8.9599999999999902</v>
       </c>
       <c r="J65" t="s">
         <v>45</v>
@@ -2796,7 +2818,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="66" spans="1:11">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -2831,7 +2853,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="67" spans="1:11">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -2857,7 +2879,7 @@
         <v>212.7</v>
       </c>
       <c r="I67">
-        <v>9.73999999999999</v>
+        <v>9.7399999999999896</v>
       </c>
       <c r="J67" t="s">
         <v>44</v>
@@ -2866,7 +2888,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="68" spans="1:11">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -2892,7 +2914,7 @@
         <v>237.66</v>
       </c>
       <c r="I68">
-        <v>9.81999999999999</v>
+        <v>9.8199999999999896</v>
       </c>
       <c r="J68" t="s">
         <v>38</v>
@@ -2901,7 +2923,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="69" spans="1:11">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -2927,7 +2949,7 @@
         <v>239.44</v>
       </c>
       <c r="I69">
-        <v>9.88</v>
+        <v>9.8800000000000008</v>
       </c>
       <c r="J69" t="s">
         <v>36</v>
@@ -2936,7 +2958,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="70" spans="1:11">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -2971,7 +2993,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="71" spans="1:11">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -3006,7 +3028,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="72" spans="1:11">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -3041,7 +3063,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="73" spans="1:11">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -3076,7 +3098,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="1:11">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -3111,7 +3133,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="75" spans="1:11">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -3146,7 +3168,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="76" spans="1:11">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -3181,7 +3203,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="77" spans="1:11">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -3216,7 +3238,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="78" spans="1:11">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -3251,7 +3273,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="79" spans="1:11">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -3286,7 +3308,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="80" spans="1:11">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -3321,7 +3343,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="81" spans="1:11">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -3356,7 +3378,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="82" spans="1:11">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -3391,7 +3413,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="83" spans="1:11">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -3408,7 +3430,7 @@
         <v>19</v>
       </c>
       <c r="F83">
-        <v>134.48</v>
+        <v>134.47999999999999</v>
       </c>
       <c r="G83">
         <v>122.64</v>
@@ -3426,7 +3448,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="84" spans="1:11">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -3461,7 +3483,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="85" spans="1:11">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -3496,7 +3518,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="86" spans="1:11">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -3513,7 +3535,7 @@
         <v>20</v>
       </c>
       <c r="F86">
-        <v>131.64</v>
+        <v>131.63999999999999</v>
       </c>
       <c r="G86">
         <v>119.36</v>
@@ -3531,7 +3553,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="87" spans="1:11">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -3566,7 +3588,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="88" spans="1:11">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -3583,13 +3605,13 @@
         <v>17</v>
       </c>
       <c r="F88">
-        <v>134.36</v>
+        <v>134.36000000000001</v>
       </c>
       <c r="G88">
         <v>121.68</v>
       </c>
       <c r="H88">
-        <v>256.04</v>
+        <v>256.04000000000002</v>
       </c>
       <c r="I88">
         <v>12.68</v>
@@ -3601,7 +3623,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="89" spans="1:11">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -3636,7 +3658,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="90" spans="1:11">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -3671,7 +3693,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="91" spans="1:11">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -3706,7 +3728,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="92" spans="1:11">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -3723,7 +3745,7 @@
         <v>27</v>
       </c>
       <c r="F92">
-        <v>145.58</v>
+        <v>145.58000000000001</v>
       </c>
       <c r="G92">
         <v>132.66</v>
@@ -3741,7 +3763,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="93" spans="1:11">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -3776,7 +3798,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="94" spans="1:11">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -3811,7 +3833,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="95" spans="1:11">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -3846,7 +3868,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="96" spans="1:11">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -3881,7 +3903,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="97" spans="1:11">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -3916,7 +3938,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="98" spans="1:11">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -3951,7 +3973,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="99" spans="1:11">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -3968,7 +3990,7 @@
         <v>13</v>
       </c>
       <c r="F99">
-        <v>139.48</v>
+        <v>139.47999999999999</v>
       </c>
       <c r="G99">
         <v>125.28</v>
@@ -3986,7 +4008,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="100" spans="1:11">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -4006,7 +4028,7 @@
         <v>167.22</v>
       </c>
       <c r="G100">
-        <v>152.58</v>
+        <v>152.58000000000001</v>
       </c>
       <c r="H100">
         <v>319.8</v>
@@ -4021,7 +4043,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="101" spans="1:11">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -4056,7 +4078,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="102" spans="1:11">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -4091,7 +4113,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="103" spans="1:11">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -4126,7 +4148,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="104" spans="1:11">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -4161,7 +4183,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="105" spans="1:11">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -4196,7 +4218,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="106" spans="1:11">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -4231,7 +4253,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="107" spans="1:11">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -4266,7 +4288,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="108" spans="1:11">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -4283,7 +4305,7 @@
         <v>28</v>
       </c>
       <c r="F108">
-        <v>142.7</v>
+        <v>142.69999999999999</v>
       </c>
       <c r="G108">
         <v>127.04</v>
@@ -4301,7 +4323,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="109" spans="1:11">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -4336,7 +4358,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="110" spans="1:11">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -4371,7 +4393,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="111" spans="1:11">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -4406,7 +4428,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="112" spans="1:11">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -4441,7 +4463,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="113" spans="1:11">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -4476,7 +4498,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="114" spans="1:11">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -4502,7 +4524,7 @@
         <v>190.88</v>
       </c>
       <c r="I114">
-        <v>16.6</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="J114" t="s">
         <v>42</v>
@@ -4511,7 +4533,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="115" spans="1:11">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -4546,7 +4568,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="116" spans="1:11">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -4572,7 +4594,7 @@
         <v>227.02</v>
       </c>
       <c r="I116">
-        <v>16.94</v>
+        <v>16.940000000000001</v>
       </c>
       <c r="J116" t="s">
         <v>38</v>
@@ -4581,7 +4603,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="117" spans="1:11">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -4607,7 +4629,7 @@
         <v>209.4</v>
       </c>
       <c r="I117">
-        <v>17.6</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="J117" t="s">
         <v>40</v>
@@ -4616,7 +4638,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="118" spans="1:11">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -4642,7 +4664,7 @@
         <v>245.4</v>
       </c>
       <c r="I118">
-        <v>17.6</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="J118" t="s">
         <v>35</v>
@@ -4651,7 +4673,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="119" spans="1:11">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -4677,7 +4699,7 @@
         <v>193.5</v>
       </c>
       <c r="I119">
-        <v>17.74</v>
+        <v>17.739999999999998</v>
       </c>
       <c r="J119" t="s">
         <v>41</v>
@@ -4686,7 +4708,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="120" spans="1:11">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -4712,7 +4734,7 @@
         <v>267.74</v>
       </c>
       <c r="I120">
-        <v>17.74</v>
+        <v>17.739999999999998</v>
       </c>
       <c r="J120" t="s">
         <v>39</v>
@@ -4721,7 +4743,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="121" spans="1:11">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -4747,7 +4769,7 @@
         <v>197.56</v>
       </c>
       <c r="I121">
-        <v>18.08</v>
+        <v>18.079999999999998</v>
       </c>
       <c r="J121" t="s">
         <v>34</v>
@@ -4756,7 +4778,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="122" spans="1:11">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -4782,7 +4804,7 @@
         <v>163.9</v>
       </c>
       <c r="I122">
-        <v>18.58</v>
+        <v>18.579999999999998</v>
       </c>
       <c r="J122" t="s">
         <v>35</v>
@@ -4791,7 +4813,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="123" spans="1:11">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -4811,7 +4833,7 @@
         <v>99.58</v>
       </c>
       <c r="G123">
-        <v>80.96</v>
+        <v>80.959999999999994</v>
       </c>
       <c r="H123">
         <v>180.54</v>
@@ -4826,7 +4848,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="124" spans="1:11">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -4861,7 +4883,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="125" spans="1:11">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -4896,7 +4918,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="126" spans="1:11">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -4922,7 +4944,7 @@
         <v>232.36</v>
       </c>
       <c r="I126">
-        <v>19.08</v>
+        <v>19.079999999999998</v>
       </c>
       <c r="J126" t="s">
         <v>39</v>
@@ -4931,7 +4953,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="127" spans="1:11">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -4948,7 +4970,7 @@
         <v>20</v>
       </c>
       <c r="F127">
-        <v>128.7</v>
+        <v>128.69999999999999</v>
       </c>
       <c r="G127">
         <v>109.54</v>
@@ -4966,7 +4988,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="128" spans="1:11">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -4992,7 +5014,7 @@
         <v>210.48</v>
       </c>
       <c r="I128">
-        <v>19.44</v>
+        <v>19.440000000000001</v>
       </c>
       <c r="J128" t="s">
         <v>44</v>
@@ -5001,7 +5023,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="129" spans="1:11">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -5036,7 +5058,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="130" spans="1:11">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -5071,7 +5093,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="131" spans="1:11">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -5106,7 +5128,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="132" spans="1:11">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -5126,13 +5148,13 @@
         <v>93.02</v>
       </c>
       <c r="G132">
-        <v>73.1</v>
+        <v>73.099999999999994</v>
       </c>
       <c r="H132">
         <v>166.12</v>
       </c>
       <c r="I132">
-        <v>19.92</v>
+        <v>19.920000000000002</v>
       </c>
       <c r="J132" t="s">
         <v>38</v>
@@ -5141,7 +5163,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="133" spans="1:11">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -5176,7 +5198,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="134" spans="1:11">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -5211,7 +5233,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="135" spans="1:11">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -5246,7 +5268,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="136" spans="1:11">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -5281,7 +5303,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="137" spans="1:11">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -5316,7 +5338,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="138" spans="1:11">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -5351,7 +5373,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="139" spans="1:11">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -5386,7 +5408,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="140" spans="1:11">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -5421,7 +5443,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="141" spans="1:11">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -5456,7 +5478,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="142" spans="1:11">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -5491,7 +5513,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="143" spans="1:11">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -5526,7 +5548,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="144" spans="1:11">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -5561,7 +5583,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="145" spans="1:11">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -5596,7 +5618,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="146" spans="1:11">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
         <v>144</v>
       </c>
@@ -5631,7 +5653,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="147" spans="1:11">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -5666,7 +5688,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="148" spans="1:11">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
         <v>146</v>
       </c>
@@ -5701,7 +5723,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="149" spans="1:11">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -5721,7 +5743,7 @@
         <v>98.36</v>
       </c>
       <c r="G149">
-        <v>74.96</v>
+        <v>74.959999999999994</v>
       </c>
       <c r="H149">
         <v>173.32</v>
@@ -5736,7 +5758,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="150" spans="1:11">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -5771,7 +5793,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="151" spans="1:11">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
         <v>149</v>
       </c>
@@ -5806,7 +5828,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="152" spans="1:11">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
         <v>150</v>
       </c>
@@ -5841,7 +5863,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="153" spans="1:11">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
         <v>151</v>
       </c>
@@ -5876,7 +5898,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="154" spans="1:11">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
         <v>152</v>
       </c>
@@ -5911,7 +5933,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="155" spans="1:11">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
         <v>153</v>
       </c>
@@ -5931,7 +5953,7 @@
         <v>96.22</v>
       </c>
       <c r="G155">
-        <v>70.68</v>
+        <v>70.680000000000007</v>
       </c>
       <c r="H155">
         <v>166.9</v>
@@ -5946,7 +5968,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="156" spans="1:11">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
         <v>154</v>
       </c>
@@ -5981,7 +6003,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="157" spans="1:11">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
         <v>155</v>
       </c>
@@ -6016,7 +6038,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="158" spans="1:11">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
         <v>156</v>
       </c>
@@ -6051,7 +6073,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="159" spans="1:11">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
         <v>157</v>
       </c>
@@ -6086,7 +6108,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="160" spans="1:11">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
         <v>158</v>
       </c>
@@ -6121,7 +6143,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="161" spans="1:11">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
         <v>159</v>
       </c>
@@ -6156,7 +6178,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="162" spans="1:11">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
         <v>160</v>
       </c>
@@ -6191,7 +6213,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="163" spans="1:11">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
         <v>161</v>
       </c>
@@ -6226,7 +6248,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="164" spans="1:11">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
         <v>162</v>
       </c>
@@ -6261,7 +6283,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="165" spans="1:11">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
         <v>163</v>
       </c>
@@ -6296,7 +6318,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="166" spans="1:11">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
         <v>164</v>
       </c>
@@ -6331,7 +6353,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="167" spans="1:11">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
         <v>165</v>
       </c>
@@ -6366,7 +6388,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="168" spans="1:11">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
         <v>166</v>
       </c>
@@ -6401,7 +6423,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="169" spans="1:11">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
         <v>167</v>
       </c>
@@ -6436,7 +6458,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="170" spans="1:11">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
         <v>168</v>
       </c>
@@ -6471,7 +6493,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="171" spans="1:11">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
         <v>169</v>
       </c>
@@ -6506,7 +6528,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="172" spans="1:11">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
         <v>170</v>
       </c>
@@ -6541,7 +6563,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="173" spans="1:11">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
         <v>171</v>
       </c>
@@ -6558,7 +6580,7 @@
         <v>20</v>
       </c>
       <c r="F173">
-        <v>148.02</v>
+        <v>148.02000000000001</v>
       </c>
       <c r="G173">
         <v>118.3</v>
@@ -6576,7 +6598,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="174" spans="1:11">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
         <v>172</v>
       </c>
@@ -6611,7 +6633,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="175" spans="1:11">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
         <v>173</v>
       </c>
@@ -6646,7 +6668,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="176" spans="1:11">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
         <v>174</v>
       </c>
@@ -6681,7 +6703,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="177" spans="1:11">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
         <v>175</v>
       </c>
@@ -6716,7 +6738,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="178" spans="1:11">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
         <v>176</v>
       </c>
@@ -6751,7 +6773,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="179" spans="1:11">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
         <v>177</v>
       </c>
@@ -6777,7 +6799,7 @@
         <v>242.36</v>
       </c>
       <c r="I179">
-        <v>32.16</v>
+        <v>32.159999999999997</v>
       </c>
       <c r="J179" t="s">
         <v>34</v>
@@ -6786,7 +6808,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="180" spans="1:11">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
         <v>178</v>
       </c>
@@ -6821,7 +6843,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="181" spans="1:11">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
         <v>179</v>
       </c>
@@ -6856,7 +6878,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="182" spans="1:11">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
         <v>180</v>
       </c>
@@ -6873,7 +6895,7 @@
         <v>22</v>
       </c>
       <c r="F182">
-        <v>129.8</v>
+        <v>129.80000000000001</v>
       </c>
       <c r="G182">
         <v>96.06</v>
@@ -6891,7 +6913,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="183" spans="1:11">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
         <v>181</v>
       </c>
@@ -6926,7 +6948,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="184" spans="1:11">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
         <v>182</v>
       </c>
@@ -6952,7 +6974,7 @@
         <v>254.04</v>
       </c>
       <c r="I184">
-        <v>33.88</v>
+        <v>33.880000000000003</v>
       </c>
       <c r="J184" t="s">
         <v>34</v>
@@ -6961,7 +6983,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="185" spans="1:11">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
         <v>183</v>
       </c>
@@ -6996,7 +7018,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="186" spans="1:11">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
         <v>184</v>
       </c>
@@ -7031,7 +7053,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="187" spans="1:11">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
         <v>185</v>
       </c>
@@ -7057,7 +7079,7 @@
         <v>212.2</v>
       </c>
       <c r="I187">
-        <v>35.12</v>
+        <v>35.119999999999997</v>
       </c>
       <c r="J187" t="s">
         <v>45</v>
@@ -7066,7 +7088,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="188" spans="1:11">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
         <v>186</v>
       </c>
@@ -7101,7 +7123,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="189" spans="1:11">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
         <v>187</v>
       </c>
@@ -7118,7 +7140,7 @@
         <v>30</v>
       </c>
       <c r="F189">
-        <v>144.08</v>
+        <v>144.08000000000001</v>
       </c>
       <c r="G189">
         <v>108.92</v>
@@ -7127,7 +7149,7 @@
         <v>253</v>
       </c>
       <c r="I189">
-        <v>35.16</v>
+        <v>35.159999999999997</v>
       </c>
       <c r="J189" t="s">
         <v>40</v>
@@ -7136,7 +7158,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="190" spans="1:11">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
         <v>188</v>
       </c>
@@ -7159,7 +7181,7 @@
         <v>114.86</v>
       </c>
       <c r="H190">
-        <v>264.96</v>
+        <v>264.95999999999998</v>
       </c>
       <c r="I190">
         <v>35.24</v>
@@ -7171,7 +7193,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="191" spans="1:11">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
         <v>189</v>
       </c>
@@ -7197,7 +7219,7 @@
         <v>281.5</v>
       </c>
       <c r="I191">
-        <v>35.38</v>
+        <v>35.380000000000003</v>
       </c>
       <c r="J191" t="s">
         <v>46</v>
@@ -7206,7 +7228,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="192" spans="1:11">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
         <v>190</v>
       </c>
@@ -7226,13 +7248,13 @@
         <v>117.02</v>
       </c>
       <c r="G192">
-        <v>81.54</v>
+        <v>81.540000000000006</v>
       </c>
       <c r="H192">
         <v>198.56</v>
       </c>
       <c r="I192">
-        <v>35.48</v>
+        <v>35.479999999999997</v>
       </c>
       <c r="J192" t="s">
         <v>44</v>
@@ -7241,7 +7263,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="193" spans="1:11">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
         <v>191</v>
       </c>
@@ -7258,7 +7280,7 @@
         <v>18</v>
       </c>
       <c r="F193">
-        <v>145.14</v>
+        <v>145.13999999999999</v>
       </c>
       <c r="G193">
         <v>109.08</v>
@@ -7276,7 +7298,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="194" spans="1:11">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
         <v>192</v>
       </c>
@@ -7299,7 +7321,7 @@
         <v>118.82</v>
       </c>
       <c r="H194">
-        <v>273.78</v>
+        <v>273.77999999999997</v>
       </c>
       <c r="I194">
         <v>36.14</v>
@@ -7311,7 +7333,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="195" spans="1:11">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
         <v>193</v>
       </c>
@@ -7346,7 +7368,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="196" spans="1:11">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
         <v>194</v>
       </c>
@@ -7372,7 +7394,7 @@
         <v>258.42</v>
       </c>
       <c r="I196">
-        <v>37.34</v>
+        <v>37.340000000000003</v>
       </c>
       <c r="J196" t="s">
         <v>41</v>
@@ -7381,7 +7403,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="197" spans="1:11">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
         <v>195</v>
       </c>
@@ -7416,7 +7438,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="198" spans="1:11">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
         <v>196</v>
       </c>
@@ -7451,7 +7473,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="199" spans="1:11">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
         <v>197</v>
       </c>
@@ -7486,7 +7508,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="200" spans="1:11">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
         <v>198</v>
       </c>
@@ -7521,7 +7543,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="201" spans="1:11">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
         <v>199</v>
       </c>
@@ -7547,7 +7569,7 @@
         <v>232.26</v>
       </c>
       <c r="I201">
-        <v>39.38</v>
+        <v>39.380000000000003</v>
       </c>
       <c r="J201" t="s">
         <v>39</v>
@@ -7556,7 +7578,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="202" spans="1:11">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
         <v>200</v>
       </c>
@@ -7576,13 +7598,13 @@
         <v>113.94</v>
       </c>
       <c r="G202">
-        <v>74.46</v>
+        <v>74.459999999999994</v>
       </c>
       <c r="H202">
         <v>188.4</v>
       </c>
       <c r="I202">
-        <v>39.48</v>
+        <v>39.479999999999997</v>
       </c>
       <c r="J202" t="s">
         <v>44</v>
@@ -7591,7 +7613,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="203" spans="1:11">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
         <v>201</v>
       </c>
@@ -7617,7 +7639,7 @@
         <v>196.2</v>
       </c>
       <c r="I203">
-        <v>39.88</v>
+        <v>39.880000000000003</v>
       </c>
       <c r="J203" t="s">
         <v>40</v>
@@ -7626,7 +7648,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="204" spans="1:11">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
         <v>202</v>
       </c>
@@ -7661,7 +7683,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="205" spans="1:11">
+    <row r="205" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
         <v>203</v>
       </c>
@@ -7696,7 +7718,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="206" spans="1:11">
+    <row r="206" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A206" s="1">
         <v>204</v>
       </c>
@@ -7731,7 +7753,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="207" spans="1:11">
+    <row r="207" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
         <v>205</v>
       </c>
@@ -7751,7 +7773,7 @@
         <v>106.86</v>
       </c>
       <c r="G207">
-        <v>65.1</v>
+        <v>65.099999999999994</v>
       </c>
       <c r="H207">
         <v>171.96</v>
@@ -7766,7 +7788,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="208" spans="1:11">
+    <row r="208" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A208" s="1">
         <v>206</v>
       </c>
@@ -7786,7 +7808,7 @@
         <v>115.58</v>
       </c>
       <c r="G208">
-        <v>73.24</v>
+        <v>73.239999999999995</v>
       </c>
       <c r="H208">
         <v>188.82</v>
@@ -7801,7 +7823,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="209" spans="1:11">
+    <row r="209" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A209" s="1">
         <v>207</v>
       </c>
@@ -7836,7 +7858,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="210" spans="1:11">
+    <row r="210" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A210" s="1">
         <v>208</v>
       </c>
@@ -7871,7 +7893,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="211" spans="1:11">
+    <row r="211" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
         <v>209</v>
       </c>
@@ -7906,7 +7928,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="212" spans="1:11">
+    <row r="212" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A212" s="1">
         <v>210</v>
       </c>
@@ -7929,7 +7951,7 @@
         <v>127.5</v>
       </c>
       <c r="H212">
-        <v>298.22</v>
+        <v>298.22000000000003</v>
       </c>
       <c r="I212">
         <v>43.22</v>
@@ -7941,7 +7963,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="213" spans="1:11">
+    <row r="213" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
         <v>211</v>
       </c>
@@ -7976,7 +7998,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="214" spans="1:11">
+    <row r="214" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A214" s="1">
         <v>212</v>
       </c>
@@ -7993,7 +8015,7 @@
         <v>16</v>
       </c>
       <c r="F214">
-        <v>153.86</v>
+        <v>153.86000000000001</v>
       </c>
       <c r="G214">
         <v>110.14</v>
@@ -8011,7 +8033,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="215" spans="1:11">
+    <row r="215" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A215" s="1">
         <v>213</v>
       </c>
@@ -8028,7 +8050,7 @@
         <v>29</v>
       </c>
       <c r="F215">
-        <v>142.64</v>
+        <v>142.63999999999999</v>
       </c>
       <c r="G215">
         <v>98.84</v>
@@ -8046,7 +8068,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="216" spans="1:11">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
         <v>214</v>
       </c>
@@ -8081,7 +8103,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="217" spans="1:11">
+    <row r="217" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
         <v>215</v>
       </c>
@@ -8116,7 +8138,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="218" spans="1:11">
+    <row r="218" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
         <v>216</v>
       </c>
@@ -8133,7 +8155,7 @@
         <v>23</v>
       </c>
       <c r="F218">
-        <v>146.64</v>
+        <v>146.63999999999999</v>
       </c>
       <c r="G218">
         <v>101.4</v>
@@ -8151,7 +8173,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="219" spans="1:11">
+    <row r="219" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A219" s="1">
         <v>217</v>
       </c>
@@ -8168,7 +8190,7 @@
         <v>24</v>
       </c>
       <c r="F219">
-        <v>137.42</v>
+        <v>137.41999999999999</v>
       </c>
       <c r="G219">
         <v>92.16</v>
@@ -8186,7 +8208,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="220" spans="1:11">
+    <row r="220" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A220" s="1">
         <v>218</v>
       </c>
@@ -8221,7 +8243,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="221" spans="1:11">
+    <row r="221" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
         <v>219</v>
       </c>
@@ -8256,7 +8278,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="222" spans="1:11">
+    <row r="222" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A222" s="1">
         <v>220</v>
       </c>
@@ -8273,7 +8295,7 @@
         <v>29</v>
       </c>
       <c r="F222">
-        <v>130.8</v>
+        <v>130.80000000000001</v>
       </c>
       <c r="G222">
         <v>84.5</v>
@@ -8291,7 +8313,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="223" spans="1:11">
+    <row r="223" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A223" s="1">
         <v>221</v>
       </c>
@@ -8326,7 +8348,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="224" spans="1:11">
+    <row r="224" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A224" s="1">
         <v>222</v>
       </c>
@@ -8361,7 +8383,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="225" spans="1:11">
+    <row r="225" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A225" s="1">
         <v>223</v>
       </c>
@@ -8384,7 +8406,7 @@
         <v>114.82</v>
       </c>
       <c r="H225">
-        <v>277.04</v>
+        <v>277.04000000000002</v>
       </c>
       <c r="I225">
         <v>47.4</v>
@@ -8396,7 +8418,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="226" spans="1:11">
+    <row r="226" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A226" s="1">
         <v>224</v>
       </c>
@@ -8431,7 +8453,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="227" spans="1:11">
+    <row r="227" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A227" s="1">
         <v>225</v>
       </c>
@@ -8448,7 +8470,7 @@
         <v>21</v>
       </c>
       <c r="F227">
-        <v>139.92</v>
+        <v>139.91999999999999</v>
       </c>
       <c r="G227">
         <v>91.84</v>
@@ -8466,7 +8488,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="228" spans="1:11">
+    <row r="228" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A228" s="1">
         <v>226</v>
       </c>
@@ -8483,7 +8505,7 @@
         <v>20</v>
       </c>
       <c r="F228">
-        <v>151.36</v>
+        <v>151.36000000000001</v>
       </c>
       <c r="G228">
         <v>103.22</v>
@@ -8501,7 +8523,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="229" spans="1:11">
+    <row r="229" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A229" s="1">
         <v>227</v>
       </c>
@@ -8518,7 +8540,7 @@
         <v>15</v>
       </c>
       <c r="F229">
-        <v>147.8</v>
+        <v>147.80000000000001</v>
       </c>
       <c r="G229">
         <v>98.98</v>
@@ -8536,7 +8558,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="230" spans="1:11">
+    <row r="230" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A230" s="1">
         <v>228</v>
       </c>
@@ -8571,7 +8593,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="231" spans="1:11">
+    <row r="231" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A231" s="1">
         <v>229</v>
       </c>
@@ -8591,7 +8613,7 @@
         <v>187.22</v>
       </c>
       <c r="G231">
-        <v>137.92</v>
+        <v>137.91999999999999</v>
       </c>
       <c r="H231">
         <v>325.14</v>
@@ -8606,7 +8628,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="232" spans="1:11">
+    <row r="232" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A232" s="1">
         <v>230</v>
       </c>
@@ -8641,7 +8663,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="233" spans="1:11">
+    <row r="233" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A233" s="1">
         <v>231</v>
       </c>
@@ -8676,7 +8698,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="234" spans="1:11">
+    <row r="234" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A234" s="1">
         <v>232</v>
       </c>
@@ -8711,7 +8733,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="235" spans="1:11">
+    <row r="235" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A235" s="1">
         <v>233</v>
       </c>
@@ -8746,7 +8768,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="236" spans="1:11">
+    <row r="236" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A236" s="1">
         <v>234</v>
       </c>
@@ -8781,7 +8803,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="237" spans="1:11">
+    <row r="237" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A237" s="1">
         <v>235</v>
       </c>
@@ -8816,7 +8838,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="238" spans="1:11">
+    <row r="238" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A238" s="1">
         <v>236</v>
       </c>
@@ -8851,7 +8873,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="239" spans="1:11">
+    <row r="239" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A239" s="1">
         <v>237</v>
       </c>
@@ -8886,7 +8908,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="240" spans="1:11">
+    <row r="240" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A240" s="1">
         <v>238</v>
       </c>
@@ -8903,7 +8925,7 @@
         <v>17</v>
       </c>
       <c r="F240">
-        <v>150.08</v>
+        <v>150.08000000000001</v>
       </c>
       <c r="G240">
         <v>97.56</v>
@@ -8921,7 +8943,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="241" spans="1:11">
+    <row r="241" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A241" s="1">
         <v>239</v>
       </c>
@@ -8956,7 +8978,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="242" spans="1:11">
+    <row r="242" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A242" s="1">
         <v>240</v>
       </c>
@@ -8991,7 +9013,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="243" spans="1:11">
+    <row r="243" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A243" s="1">
         <v>241</v>
       </c>
@@ -9026,7 +9048,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="244" spans="1:11">
+    <row r="244" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A244" s="1">
         <v>242</v>
       </c>
@@ -9061,7 +9083,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="245" spans="1:11">
+    <row r="245" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A245" s="1">
         <v>243</v>
       </c>
@@ -9096,7 +9118,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="246" spans="1:11">
+    <row r="246" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A246" s="1">
         <v>244</v>
       </c>
@@ -9119,7 +9141,7 @@
         <v>103.78</v>
       </c>
       <c r="H246">
-        <v>263.6</v>
+        <v>263.60000000000002</v>
       </c>
       <c r="I246">
         <v>56.04</v>
@@ -9131,7 +9153,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="247" spans="1:11">
+    <row r="247" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A247" s="1">
         <v>245</v>
       </c>
@@ -9166,7 +9188,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="248" spans="1:11">
+    <row r="248" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A248" s="1">
         <v>246</v>
       </c>
@@ -9201,7 +9223,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="249" spans="1:11">
+    <row r="249" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A249" s="1">
         <v>247</v>
       </c>
@@ -9236,7 +9258,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="250" spans="1:11">
+    <row r="250" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A250" s="1">
         <v>248</v>
       </c>
@@ -9253,7 +9275,7 @@
         <v>22</v>
       </c>
       <c r="F250">
-        <v>137.52</v>
+        <v>137.52000000000001</v>
       </c>
       <c r="G250">
         <v>77.8</v>
@@ -9271,7 +9293,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="251" spans="1:11">
+    <row r="251" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A251" s="1">
         <v>249</v>
       </c>
@@ -9288,7 +9310,7 @@
         <v>21</v>
       </c>
       <c r="F251">
-        <v>129.86</v>
+        <v>129.86000000000001</v>
       </c>
       <c r="G251">
         <v>68.8</v>
@@ -9306,7 +9328,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="252" spans="1:11">
+    <row r="252" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A252" s="1">
         <v>250</v>
       </c>
@@ -9323,13 +9345,13 @@
         <v>13</v>
       </c>
       <c r="F252">
-        <v>163.2</v>
+        <v>163.19999999999999</v>
       </c>
       <c r="G252">
         <v>101.2</v>
       </c>
       <c r="H252">
-        <v>264.4</v>
+        <v>264.39999999999998</v>
       </c>
       <c r="I252">
         <v>62</v>
@@ -9341,7 +9363,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="253" spans="1:11">
+    <row r="253" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A253" s="1">
         <v>251</v>
       </c>
@@ -9376,7 +9398,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="254" spans="1:11">
+    <row r="254" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A254" s="1">
         <v>252</v>
       </c>
@@ -9396,7 +9418,7 @@
         <v>143.22</v>
       </c>
       <c r="G254">
-        <v>80.68</v>
+        <v>80.680000000000007</v>
       </c>
       <c r="H254">
         <v>223.9</v>
@@ -9411,7 +9433,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="255" spans="1:11">
+    <row r="255" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A255" s="1">
         <v>253</v>
       </c>
@@ -9446,7 +9468,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="256" spans="1:11">
+    <row r="256" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A256" s="1">
         <v>254</v>
       </c>
@@ -9481,7 +9503,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="257" spans="1:11">
+    <row r="257" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A257" s="1">
         <v>255</v>
       </c>
@@ -9501,7 +9523,7 @@
         <v>135.88</v>
       </c>
       <c r="G257">
-        <v>71.74</v>
+        <v>71.739999999999995</v>
       </c>
       <c r="H257">
         <v>207.62</v>
@@ -9516,7 +9538,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="258" spans="1:11">
+    <row r="258" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A258" s="1">
         <v>256</v>
       </c>
@@ -9542,7 +9564,7 @@
         <v>237.84</v>
       </c>
       <c r="I258">
-        <v>64.68</v>
+        <v>64.680000000000007</v>
       </c>
       <c r="J258" t="s">
         <v>46</v>
@@ -9551,7 +9573,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="259" spans="1:11">
+    <row r="259" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A259" s="1">
         <v>257</v>
       </c>
@@ -9586,7 +9608,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="260" spans="1:11">
+    <row r="260" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A260" s="1">
         <v>258</v>
       </c>
@@ -9606,7 +9628,7 @@
         <v>130.1</v>
       </c>
       <c r="G260">
-        <v>64.6</v>
+        <v>64.599999999999994</v>
       </c>
       <c r="H260">
         <v>194.7</v>
@@ -9621,7 +9643,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="261" spans="1:11">
+    <row r="261" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A261" s="1">
         <v>259</v>
       </c>
@@ -9656,7 +9678,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="262" spans="1:11">
+    <row r="262" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A262" s="1">
         <v>260</v>
       </c>
@@ -9691,7 +9713,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="263" spans="1:11">
+    <row r="263" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A263" s="1">
         <v>261</v>
       </c>
@@ -9726,7 +9748,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="264" spans="1:11">
+    <row r="264" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A264" s="1">
         <v>262</v>
       </c>
@@ -9761,7 +9783,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="265" spans="1:11">
+    <row r="265" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A265" s="1">
         <v>263</v>
       </c>
@@ -9784,7 +9806,7 @@
         <v>102.14</v>
       </c>
       <c r="H265">
-        <v>271.16</v>
+        <v>271.16000000000003</v>
       </c>
       <c r="I265">
         <v>66.88</v>
@@ -9796,7 +9818,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="266" spans="1:11">
+    <row r="266" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A266" s="1">
         <v>264</v>
       </c>
@@ -9831,7 +9853,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="267" spans="1:11">
+    <row r="267" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A267" s="1">
         <v>265</v>
       </c>
@@ -9866,7 +9888,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="268" spans="1:11">
+    <row r="268" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A268" s="1">
         <v>266</v>
       </c>
@@ -9889,7 +9911,7 @@
         <v>95.62</v>
       </c>
       <c r="H268">
-        <v>259.22</v>
+        <v>259.22000000000003</v>
       </c>
       <c r="I268">
         <v>67.98</v>
@@ -9901,7 +9923,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="269" spans="1:11">
+    <row r="269" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A269" s="1">
         <v>267</v>
       </c>
@@ -9918,7 +9940,7 @@
         <v>16</v>
       </c>
       <c r="F269">
-        <v>149.98</v>
+        <v>149.97999999999999</v>
       </c>
       <c r="G269">
         <v>81.28</v>
@@ -9936,7 +9958,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="270" spans="1:11">
+    <row r="270" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A270" s="1">
         <v>268</v>
       </c>
@@ -9959,10 +9981,10 @@
         <v>95.34</v>
       </c>
       <c r="H270">
-        <v>259.72</v>
+        <v>259.72000000000003</v>
       </c>
       <c r="I270">
-        <v>69.04</v>
+        <v>69.040000000000006</v>
       </c>
       <c r="J270" t="s">
         <v>43</v>
@@ -9971,7 +9993,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="271" spans="1:11">
+    <row r="271" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A271" s="1">
         <v>269</v>
       </c>
@@ -10006,7 +10028,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="272" spans="1:11">
+    <row r="272" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A272" s="1">
         <v>270</v>
       </c>
@@ -10032,7 +10054,7 @@
         <v>227.38</v>
       </c>
       <c r="I272">
-        <v>70.1</v>
+        <v>70.099999999999994</v>
       </c>
       <c r="J272" t="s">
         <v>41</v>
@@ -10041,7 +10063,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="273" spans="1:11">
+    <row r="273" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A273" s="1">
         <v>271</v>
       </c>
@@ -10076,7 +10098,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="274" spans="1:11">
+    <row r="274" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A274" s="1">
         <v>272</v>
       </c>
@@ -10096,7 +10118,7 @@
         <v>153.4</v>
       </c>
       <c r="G274">
-        <v>77.6</v>
+        <v>77.599999999999994</v>
       </c>
       <c r="H274">
         <v>231</v>
@@ -10111,7 +10133,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="275" spans="1:11">
+    <row r="275" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A275" s="1">
         <v>273</v>
       </c>
@@ -10128,7 +10150,7 @@
         <v>26</v>
       </c>
       <c r="F275">
-        <v>147.7</v>
+        <v>147.69999999999999</v>
       </c>
       <c r="G275">
         <v>66.16</v>
@@ -10137,7 +10159,7 @@
         <v>213.86</v>
       </c>
       <c r="I275">
-        <v>81.54</v>
+        <v>81.540000000000006</v>
       </c>
       <c r="J275" t="s">
         <v>42</v>
@@ -10146,7 +10168,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="276" spans="1:11">
+    <row r="276" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A276" s="1">
         <v>274</v>
       </c>
@@ -10181,7 +10203,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="277" spans="1:11">
+    <row r="277" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A277" s="1">
         <v>275</v>
       </c>
@@ -10198,7 +10220,7 @@
         <v>20</v>
       </c>
       <c r="F277">
-        <v>145.08</v>
+        <v>145.08000000000001</v>
       </c>
       <c r="G277">
         <v>58.28</v>
@@ -10216,7 +10238,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="278" spans="1:11">
+    <row r="278" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A278" s="1">
         <v>276</v>
       </c>
@@ -10233,10 +10255,10 @@
         <v>30</v>
       </c>
       <c r="F278">
-        <v>161.52</v>
+        <v>161.52000000000001</v>
       </c>
       <c r="G278">
-        <v>70.76</v>
+        <v>70.760000000000005</v>
       </c>
       <c r="H278">
         <v>232.28</v>
@@ -10251,7 +10273,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="279" spans="1:11">
+    <row r="279" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A279" s="1">
         <v>277</v>
       </c>
@@ -10286,7 +10308,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="280" spans="1:11">
+    <row r="280" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A280" s="1">
         <v>278</v>
       </c>
@@ -10321,7 +10343,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="281" spans="1:11">
+    <row r="281" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A281" s="1">
         <v>279</v>
       </c>
@@ -10338,7 +10360,7 @@
         <v>18</v>
       </c>
       <c r="F281">
-        <v>163.8</v>
+        <v>163.80000000000001</v>
       </c>
       <c r="G281">
         <v>51.38</v>
@@ -10357,6 +10379,18 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>